<commit_message>
skill system, collision intersect, bullet system
</commit_message>
<xml_diff>
--- a/Unity/Assets/Config/Excel/StartConfig/Release/StartMachineConfig@s.xlsx
+++ b/Unity/Assets/Config/Excel/StartConfig/Release/StartMachineConfig@s.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Nova\Legends-Of-Heroes\Unity\Assets\Config\Excel\StartConfig\Release\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C4D206-EEDD-4464-BB7A-8C71DF8C7437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F503600-7393-4DF1-8E34-A0D06D5B9419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5490" yWindow="5310" windowWidth="24285" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10650" yWindow="5865" windowWidth="24285" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StartMachineConfig" sheetId="1" r:id="rId1"/>
@@ -443,7 +443,8 @@
   <cols>
     <col min="1" max="1" width="21.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
-    <col min="3" max="5" width="12.5703125" style="3" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16" style="3" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>

</xml_diff>